<commit_message>
Uploaded the revised Event table
</commit_message>
<xml_diff>
--- a/Documentation/EVENT TABLE .xlsx
+++ b/Documentation/EVENT TABLE .xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Desktop\H-Escalation\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
   <si>
     <t xml:space="preserve">Event </t>
   </si>
@@ -44,39 +44,18 @@
     <t>Destination</t>
   </si>
   <si>
-    <t>Service ticket has reach time limit</t>
-  </si>
-  <si>
     <t xml:space="preserve">Service Request and Report System </t>
   </si>
   <si>
     <t>Escalation Management Module has an escalated ticket</t>
   </si>
   <si>
-    <t xml:space="preserve">Transform service ticket into escalation ticket </t>
-  </si>
-  <si>
     <t xml:space="preserve">Escalated Ticket </t>
   </si>
   <si>
     <t xml:space="preserve">Escalated Ticket Data Store </t>
   </si>
   <si>
-    <t xml:space="preserve">Updates of escalated ticket details </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Escalation Management Module </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Escalation Management Module sends an update of escalated ticket details to the escalation level employee </t>
-  </si>
-  <si>
-    <t xml:space="preserve">View updated escalated ticket details </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Updated escalated ticket details </t>
-  </si>
-  <si>
     <t>Escalated Ticket Status</t>
   </si>
   <si>
@@ -101,12 +80,6 @@
     <t>Supervisor/Department Manager/Resident Manager/General Manager updated escalated ticket status</t>
   </si>
   <si>
-    <t xml:space="preserve">Supervisor/Department Manager/Resident Manager/General Manager input reason for escalated ticket </t>
-  </si>
-  <si>
-    <t>Input escalated ticket's reason</t>
-  </si>
-  <si>
     <t>Reason for escalation</t>
   </si>
   <si>
@@ -150,6 +123,18 @@
   </si>
   <si>
     <t xml:space="preserve">Notification and Escalated Ticket assignment details </t>
+  </si>
+  <si>
+    <t>Transforms service ticket ino an escalation ticket</t>
+  </si>
+  <si>
+    <t>Receive Escalated Ticket</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supervisor/Department Manager/Resident Manager/General Manager enter reason for escalated ticket </t>
+  </si>
+  <si>
+    <t>Enter escalated ticket's reason</t>
   </si>
 </sst>
 </file>
@@ -185,7 +170,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -204,6 +189,24 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDE3F7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -219,7 +222,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -228,9 +231,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -244,15 +244,36 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -279,6 +300,12 @@
         <family val="1"/>
         <scheme val="none"/>
       </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -397,6 +424,11 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFDDE3F7"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -409,8 +441,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C48BE6EA-188F-4D95-8676-52EF7F071B47}" name="Table3" displayName="Table3" ref="A1:F9" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1" headerRowCellStyle="60% - Accent5">
-  <autoFilter ref="A1:F9" xr:uid="{7C6E260B-42D0-4C99-991C-B5861D492F7C}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C48BE6EA-188F-4D95-8676-52EF7F071B47}" name="Table3" displayName="Table3" ref="A1:F8" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1" headerRowCellStyle="60% - Accent5">
+  <autoFilter ref="A1:F8" xr:uid="{7C6E260B-42D0-4C99-991C-B5861D492F7C}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -727,183 +759,168 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{515E936E-83F4-471F-8CB3-4BF2B603B236}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.5703125" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" style="7" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" style="10" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" style="8" customWidth="1"/>
     <col min="4" max="6" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="6" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:6" s="5" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="1" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="F2" s="12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="64.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="18"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+    </row>
+    <row r="6" spans="1:6" s="9" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A6" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>11</v>
-      </c>
     </row>
-    <row r="3" spans="1:6" ht="77.25" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="2" t="s">
+    <row r="7" spans="1:6" ht="51.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="64.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="12" t="s">
         <v>16</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="64.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" s="11" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="C6" s="11" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="51.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="64.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>